<commit_message>
Atualização significado das labels e formulário de reomve bus trans.
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado das labels.xlsx
+++ b/WindowsApplication1/Significado das labels.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Submeter</t>
+  </si>
+  <si>
+    <t>ComboBox 9</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -522,6 +525,19 @@
       </c>
     </row>
     <row r="3" spans="1:11">
+      <c r="D3" s="4">
+        <v>42</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Bugs concertados. Remove Distr. Bus. Database adicionado
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado das labels.xlsx
+++ b/WindowsApplication1/Significado das labels.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -127,6 +127,33 @@
   </si>
   <si>
     <t>Combobox12</t>
+  </si>
+  <si>
+    <t>Distribuição/Barra/Insert</t>
+  </si>
+  <si>
+    <t>Bus Number</t>
+  </si>
+  <si>
+    <t>combobox13</t>
+  </si>
+  <si>
+    <t>textbox33</t>
+  </si>
+  <si>
+    <t>Distribuição/Barra/Remove</t>
+  </si>
+  <si>
+    <t>Bus.Case</t>
+  </si>
+  <si>
+    <t>Bus.Number</t>
+  </si>
+  <si>
+    <t>comboBox14</t>
+  </si>
+  <si>
+    <t>comboBox15</t>
   </si>
 </sst>
 </file>
@@ -537,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -898,7 +925,9 @@
       <c r="J14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1"/>
@@ -915,7 +944,125 @@
       <c r="J15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="4">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4">
+        <v>54</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="4">
+        <v>18</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
+        <v>25</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4">
+        <v>55</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="4">
+        <v>18</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4">
+        <v>26</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="1">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="1">
+        <v>56</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="1">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1">
+        <v>27</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="1">
+        <v>57</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="1">
+        <v>19</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1">
+        <v>28</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="1">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Query Distr Barra ok
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado das labels.xlsx
+++ b/WindowsApplication1/Significado das labels.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Mensagem Especial</t>
+  </si>
+  <si>
+    <t>Distr/Barra/Query</t>
+  </si>
+  <si>
+    <t>comboBox16</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,19 +247,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,53 +588,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="2.21875" customWidth="1"/>
+    <col min="8" max="8" width="2.21875" style="7" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -627,7 +645,7 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="1">
         <v>41</v>
       </c>
@@ -640,7 +658,7 @@
       <c r="G2" s="1">
         <v>15</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="1">
         <v>19</v>
       </c>
@@ -654,7 +672,7 @@
     <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="1">
         <v>42</v>
       </c>
@@ -667,7 +685,7 @@
       <c r="G3" s="1">
         <v>15</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="1">
         <v>20</v>
       </c>
@@ -679,230 +697,230 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="4">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="2">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4">
+      <c r="C4" s="6"/>
+      <c r="D4" s="2">
         <v>43</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="4">
-        <v>16</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4">
+      <c r="G4" s="2">
+        <v>16</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="2">
         <v>21</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="2">
         <v>44</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="4">
-        <v>16</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4">
+      <c r="G5" s="2">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="2">
         <v>22</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="2">
         <v>45</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="4">
-        <v>16</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="G6" s="2">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="2">
         <v>46</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="4">
-        <v>16</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="G7" s="2">
+        <v>16</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="2">
         <v>47</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="4">
-        <v>16</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="G8" s="2">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="2">
         <v>48</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="4">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="G9" s="2">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="2">
         <v>49</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="4">
-        <v>16</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="G10" s="2">
+        <v>16</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="2">
         <v>50</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="4">
-        <v>16</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="G11" s="2">
+        <v>16</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="2">
         <v>52</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="4">
-        <v>16</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="G12" s="2">
+        <v>16</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="2">
         <v>53</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="4">
-        <v>16</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="G13" s="2">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1">
@@ -911,7 +929,7 @@
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="1">
         <v>51</v>
       </c>
@@ -924,7 +942,7 @@
       <c r="G14" s="1">
         <v>17</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="1">
         <v>23</v>
       </c>
@@ -938,12 +956,12 @@
     <row r="15" spans="1:11">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="1">
         <v>24</v>
       </c>
@@ -955,60 +973,60 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="4">
+      <c r="A16" s="2">
         <v>18</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4">
+      <c r="C16" s="6"/>
+      <c r="D16" s="2">
         <v>54</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="2">
         <v>18</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4">
+      <c r="H16" s="5"/>
+      <c r="I16" s="2">
         <v>25</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="2">
         <v>55</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="2">
         <v>18</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4">
+      <c r="H17" s="5"/>
+      <c r="I17" s="2">
         <v>26</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="2">
         <v>18</v>
       </c>
     </row>
@@ -1019,7 +1037,7 @@
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="1">
         <v>56</v>
       </c>
@@ -1032,7 +1050,7 @@
       <c r="G18" s="1">
         <v>19</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="1">
         <v>27</v>
       </c>
@@ -1046,7 +1064,7 @@
     <row r="19" spans="1:11">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="1">
         <v>57</v>
       </c>
@@ -1059,7 +1077,7 @@
       <c r="G19" s="1">
         <v>19</v>
       </c>
-      <c r="H19" s="1"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="1">
         <v>28</v>
       </c>
@@ -1071,25 +1089,75 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>20</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4">
+      <c r="C20" s="6"/>
+      <c r="D20" s="2">
         <v>58</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="1">
+        <v>59</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="1">
+        <v>21</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="1">
+        <v>29</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="1">
+        <v>30</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="1">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>